<commit_message>
Added code to print schools on next line but not printing correclty yet
</commit_message>
<xml_diff>
--- a/SummerWork-2/OUTPUT.xlsx
+++ b/SummerWork-2/OUTPUT.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="All Schools Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Just School" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="414">
   <si>
     <t>Start Date</t>
   </si>
@@ -882,6 +883,382 @@
   </si>
   <si>
     <t>Cottage Grove</t>
+  </si>
+  <si>
+    <t>198.237.47.196</t>
+  </si>
+  <si>
+    <t>R_sbR4vPv2AqeWGRj</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>anna.logan@crookcounty.k12.or.us</t>
+  </si>
+  <si>
+    <t>Crook County SD</t>
+  </si>
+  <si>
+    <t>471 NE Ochoco Plaza Dr</t>
+  </si>
+  <si>
+    <t>Prineville</t>
+  </si>
+  <si>
+    <t>Duane</t>
+  </si>
+  <si>
+    <t>Yecha</t>
+  </si>
+  <si>
+    <t>duane.yecha@crookcounty.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-447-5664</t>
+  </si>
+  <si>
+    <t>541-416-9965</t>
+  </si>
+  <si>
+    <t>Director of Business and Finance</t>
+  </si>
+  <si>
+    <t>Trish</t>
+  </si>
+  <si>
+    <t>Robideau</t>
+  </si>
+  <si>
+    <t>trish.robideau@crookcounty.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-416-9966</t>
+  </si>
+  <si>
+    <t>Staff Accountant</t>
+  </si>
+  <si>
+    <t>Crook County Middle School</t>
+  </si>
+  <si>
+    <t>Suttle Lake United Methodist Camp</t>
+  </si>
+  <si>
+    <t>5 Days 4 Nights</t>
+  </si>
+  <si>
+    <t>Paulina Elementary School</t>
+  </si>
+  <si>
+    <t>Brothers Elementary School</t>
+  </si>
+  <si>
+    <t>198.237.103.59</t>
+  </si>
+  <si>
+    <t>R_2v2nE1nGeLmeQLL</t>
+  </si>
+  <si>
+    <t>Nielson</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Jennifer.nielson@adrian.k12.or.us</t>
+  </si>
+  <si>
+    <t>Adrian SD 61</t>
+  </si>
+  <si>
+    <t>PO Box 108</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Purnell</t>
+  </si>
+  <si>
+    <t>kevin.purnell@adrian.k12.or.us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin </t>
+  </si>
+  <si>
+    <t>jennifer.nielson@adrian.k12.or.us</t>
+  </si>
+  <si>
+    <t>Deputy Clerk/Business Manager</t>
+  </si>
+  <si>
+    <t>Adrian School District</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Lake Creek Campground</t>
+  </si>
+  <si>
+    <t>Prairie City</t>
+  </si>
+  <si>
+    <t>140.211.35.33</t>
+  </si>
+  <si>
+    <t>R_2dYk4qnWywoxuIa</t>
+  </si>
+  <si>
+    <t>Lakey-Campbell</t>
+  </si>
+  <si>
+    <t>Angie</t>
+  </si>
+  <si>
+    <t>angie.lakey-campbell@imblersd.org</t>
+  </si>
+  <si>
+    <t>Imbler SD 11</t>
+  </si>
+  <si>
+    <t>PO Box 164</t>
+  </si>
+  <si>
+    <t>Imbler</t>
+  </si>
+  <si>
+    <t>Teressa</t>
+  </si>
+  <si>
+    <t>Dewey</t>
+  </si>
+  <si>
+    <t>teressa.dewey@imblersd.org</t>
+  </si>
+  <si>
+    <t>Deputy Clerk</t>
+  </si>
+  <si>
+    <t>Imbler Elementary School</t>
+  </si>
+  <si>
+    <t>167.135.103.251</t>
+  </si>
+  <si>
+    <t>R_1EhCybyuCHblbGC</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>alb</t>
+  </si>
+  <si>
+    <t>x@alke.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-999-2345</t>
+  </si>
+  <si>
+    <t>541-730-2222</t>
+  </si>
+  <si>
+    <t>541-730-222</t>
+  </si>
+  <si>
+    <t>slakd</t>
+  </si>
+  <si>
+    <t>Disagree</t>
+  </si>
+  <si>
+    <t>198.237.195.8</t>
+  </si>
+  <si>
+    <t>R_2TSPHhrnuXesFMd</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>quicks@harneyesd.k12.or.us</t>
+  </si>
+  <si>
+    <t>Harney County SD 3</t>
+  </si>
+  <si>
+    <t>550 N Court Avenue</t>
+  </si>
+  <si>
+    <t>Burns</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Mckenzie</t>
+  </si>
+  <si>
+    <t>Hughes</t>
+  </si>
+  <si>
+    <t>hughesm@harneyesd.k12.or.us</t>
+  </si>
+  <si>
+    <t>541-573-6436</t>
+  </si>
+  <si>
+    <t>Teaher</t>
+  </si>
+  <si>
+    <t>Vicki</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>johnsov2@harneyesd.k12.or.us</t>
+  </si>
+  <si>
+    <t>Hines Middle School</t>
+  </si>
+  <si>
+    <t>OMSI</t>
+  </si>
+  <si>
+    <t>Outdoor Science School at the Coastal Discovery Center</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>66.154.132.120</t>
+  </si>
+  <si>
+    <t>R_3MQ1IFPflFyCs8l</t>
+  </si>
+  <si>
+    <t>VanDyke</t>
+  </si>
+  <si>
+    <t>Tera</t>
+  </si>
+  <si>
+    <t>tvandyke@nwresd.k12.or.us</t>
+  </si>
+  <si>
+    <t>Jewell SD 8</t>
+  </si>
+  <si>
+    <t>83874 Hwy 103</t>
+  </si>
+  <si>
+    <t>Seaside</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Hunsaker</t>
+  </si>
+  <si>
+    <t>aliceh@jewellk12.org</t>
+  </si>
+  <si>
+    <t>503-755-2451</t>
+  </si>
+  <si>
+    <t>terav@jewellk12.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jewell School </t>
+  </si>
+  <si>
+    <t>Camp Westwind</t>
+  </si>
+  <si>
+    <t>Lincoln City</t>
+  </si>
+  <si>
+    <t>Traveling Long Distance to Facility</t>
+  </si>
+  <si>
+    <t>2 - School Number:  [CurrentLoopNumber]Please Provide the Name:</t>
+  </si>
+  <si>
+    <t>2 - Has this school participated in any outdoor school programs before the 18-19 fiscal year?</t>
+  </si>
+  <si>
+    <t>Number of students attending Outdoor School in each grade.  Add 0 if there are no students attending in one or other grade. - 2 - 5th Grade</t>
+  </si>
+  <si>
+    <t>Number of students attending Outdoor School in each grade.  Add 0 if there are no students attending in one or other grade. - 2 - 6th Grade</t>
+  </si>
+  <si>
+    <t>2 - I certify that the student count listed above does not include students who previously attended outdoor school using Measure 99 Outdoor School Funds in 2017-2018.</t>
+  </si>
+  <si>
+    <t>Name of Outdoor School Provider for [QID9-ChoiceTextEntryValue]: - 2 - Name of Outdoor School Provider for [QID9-ChoiceTextEntryValue]: - Selected Choice</t>
+  </si>
+  <si>
+    <t>Name of Outdoor School Provider for [QID9-ChoiceTextEntryValue]: - 2 - Other - Text</t>
+  </si>
+  <si>
+    <t>Location of Camp/Facility - 2 - Name of Camp or Facility</t>
+  </si>
+  <si>
+    <t>Location of Camp/Facility - 2 - Closest City to Camp or Facility</t>
+  </si>
+  <si>
+    <t>2 - Length of Program</t>
+  </si>
+  <si>
+    <t>2 - Based on the table above, will the anticipated threshold amount per student for your program length be adequate for  [QID9-ChoiceTextEntryValue]?</t>
+  </si>
+  <si>
+    <t>2 - If threshold is enough, what do you anticipate the costs for [QID9-ChoiceTextEntryValue] being per student (please round up to whole dollar)?</t>
+  </si>
+  <si>
+    <t>Reason additional funds are needed (Check all that apply): - 2 - Reason additional funds are needed (Check all that apply): - Selected Choice</t>
+  </si>
+  <si>
+    <t>Reason additional funds are needed (Check all that apply): - 2 - Other - Text</t>
+  </si>
+  <si>
+    <t>Additional funding plans (Check all that apply): - 2 - Additional funding plans (Check all that apply): - Selected Choice</t>
+  </si>
+  <si>
+    <t>Additional funding plans (Check all that apply): - 2 - Other - Text</t>
+  </si>
+  <si>
+    <t>2 - I have reviewed the budget categories &amp; definitions and am prepared to provide a detailed budget to request for additional costs.</t>
+  </si>
+  <si>
+    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Outdoor School Provider Fees</t>
+  </si>
+  <si>
+    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Transportation</t>
+  </si>
+  <si>
+    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Personnel/Stipends</t>
+  </si>
+  <si>
+    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Program Costs incurred by District or School without administration costs</t>
+  </si>
+  <si>
+    <t>2 - Any details you would like the reviewers to consider regarding your request.</t>
+  </si>
+  <si>
+    <t>2 - [QID9-ChoiceTextEntryValue] is asking a total of  $[QID40-TotalSum] per student based on the slide table in page before.  I understand these funds are not guaranteed until I receive my Work Order and funding approval.
+While we cannot assign actual funding amounts prior to receipt of all 2018-2019 applications, the information you provided will be presented to the review team.  The review team will consider your request in conjunction with fund availability and statewide needs.  OSU will attempt to cover all or a portion of the requested funding.</t>
+  </si>
+  <si>
+    <t>2 - Although my costs are higher than the Measure 99 funding threshold, I will be using other options to fund the difference.  Therefore my application is requesting funds based on the threshold for my length of program.</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BJ12"/>
+  <dimension ref="A1:BJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1409,10 +1786,10 @@
     </row>
     <row r="2" spans="1:62">
       <c r="A2">
-        <v>43213</v>
+        <v>43213.65054398148</v>
       </c>
       <c r="B2">
-        <v>43213.66805555556</v>
+        <v>43213.66873842593</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1430,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>43213.66805555556</v>
+        <v>43213.66873842593</v>
       </c>
       <c r="I2" t="s">
         <v>63</v>
@@ -1445,10 +1822,10 @@
         <v>66</v>
       </c>
       <c r="N2">
-        <v>45.15339661</v>
+        <v>45.153396606445</v>
       </c>
       <c r="O2">
-        <v>-117.7723007</v>
+        <v>-117.77230072021</v>
       </c>
       <c r="P2" t="s">
         <v>67</v>
@@ -1555,10 +1932,10 @@
     </row>
     <row r="3" spans="1:62">
       <c r="A3">
-        <v>43213.65486111111</v>
+        <v>43213.65549768518</v>
       </c>
       <c r="B3">
-        <v>43213.67222222222</v>
+        <v>43213.67290509259</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1576,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>43213.67222222222</v>
+        <v>43213.67290509259</v>
       </c>
       <c r="I3" t="s">
         <v>87</v>
@@ -1591,10 +1968,10 @@
         <v>90</v>
       </c>
       <c r="N3">
-        <v>45.49090576</v>
+        <v>45.490905761719</v>
       </c>
       <c r="O3">
-        <v>-119.8358994</v>
+        <v>-119.83589935303</v>
       </c>
       <c r="P3" t="s">
         <v>67</v>
@@ -1701,10 +2078,10 @@
     </row>
     <row r="4" spans="1:62">
       <c r="A4">
-        <v>43213.67708333334</v>
+        <v>43213.67717592593</v>
       </c>
       <c r="B4">
-        <v>43213.67986111111</v>
+        <v>43213.67994212963</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1722,7 +2099,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>43213.67986111111</v>
+        <v>43213.67994212963</v>
       </c>
       <c r="I4" t="s">
         <v>109</v>
@@ -1737,10 +2114,10 @@
         <v>112</v>
       </c>
       <c r="N4">
-        <v>45.15339661</v>
+        <v>45.153396606445</v>
       </c>
       <c r="O4">
-        <v>-117.7723007</v>
+        <v>-117.77230072021</v>
       </c>
       <c r="P4" t="s">
         <v>67</v>
@@ -1847,10 +2224,10 @@
     </row>
     <row r="5" spans="1:62">
       <c r="A5">
-        <v>43213.69861111111</v>
+        <v>43213.69927083333</v>
       </c>
       <c r="B5">
-        <v>43213.70277777778</v>
+        <v>43213.70336805555</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1868,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>43213.70277777778</v>
+        <v>43213.70337962963</v>
       </c>
       <c r="I5" t="s">
         <v>129</v>
@@ -1883,10 +2260,10 @@
         <v>132</v>
       </c>
       <c r="N5">
-        <v>45.90289307</v>
+        <v>45.902893066406</v>
       </c>
       <c r="O5">
-        <v>-118.3401031</v>
+        <v>-118.34010314941</v>
       </c>
       <c r="P5" t="s">
         <v>67</v>
@@ -1993,10 +2370,10 @@
     </row>
     <row r="6" spans="1:62">
       <c r="A6">
-        <v>43214.37916666667</v>
+        <v>43214.37979166667</v>
       </c>
       <c r="B6">
-        <v>43214.39236111111</v>
+        <v>43214.39278935185</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -2014,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>43214.39236111111</v>
+        <v>43214.39280092593</v>
       </c>
       <c r="I6" t="s">
         <v>147</v>
@@ -2029,10 +2406,10 @@
         <v>150</v>
       </c>
       <c r="N6">
-        <v>44.26280212</v>
+        <v>44.262802124023</v>
       </c>
       <c r="O6">
-        <v>-121.226799</v>
+        <v>-121.22679901123</v>
       </c>
       <c r="P6" t="s">
         <v>67</v>
@@ -2149,209 +2526,51 @@
         <v>10</v>
       </c>
       <c r="BI6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:62">
-      <c r="A7">
-        <v>43213.67708333334</v>
-      </c>
-      <c r="B7">
-        <v>43214.425</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>64618</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>43214.425</v>
-      </c>
-      <c r="I7" t="s">
-        <v>169</v>
-      </c>
-      <c r="J7" t="s">
-        <v>170</v>
-      </c>
-      <c r="K7" t="s">
-        <v>171</v>
-      </c>
-      <c r="L7" t="s">
-        <v>172</v>
-      </c>
-      <c r="N7">
-        <v>42.53860474</v>
-      </c>
-      <c r="O7">
-        <v>-123.3478012</v>
-      </c>
-      <c r="P7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R7" t="s">
-        <v>173</v>
-      </c>
-      <c r="S7" t="s">
-        <v>174</v>
-      </c>
-      <c r="T7" t="s">
-        <v>175</v>
-      </c>
-      <c r="U7">
-        <v>97526</v>
-      </c>
-      <c r="V7" t="s">
-        <v>72</v>
-      </c>
-      <c r="W7" t="s">
-        <v>73</v>
-      </c>
-      <c r="X7">
-        <v>1</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>180</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>181</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>172</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>184</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>185</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>179</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>187</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>188</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO7">
-        <v>0</v>
-      </c>
-      <c r="AP7">
-        <v>240</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>189</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>190</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>165</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>191</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>192</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>193</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>194</v>
-      </c>
-      <c r="BJ7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:62">
       <c r="A8">
-        <v>43214.48472222222</v>
+        <v>43213.67719907407</v>
       </c>
       <c r="B8">
-        <v>43214.48819444444</v>
+        <v>43214.42510416666</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="E8">
         <v>100</v>
       </c>
       <c r="F8">
-        <v>350</v>
+        <v>64618</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>43214.48819444444</v>
+        <v>43214.42511574074</v>
       </c>
       <c r="I8" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="K8" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="L8" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="N8">
-        <v>44.03640747</v>
+        <v>42.538604736328</v>
       </c>
       <c r="O8">
-        <v>-123.0547028</v>
+        <v>-123.3478012085</v>
       </c>
       <c r="P8" t="s">
         <v>67</v>
@@ -2360,16 +2579,16 @@
         <v>68</v>
       </c>
       <c r="R8" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="S8" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="T8" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="U8">
-        <v>97426</v>
+        <v>97526</v>
       </c>
       <c r="V8" t="s">
         <v>72</v>
@@ -2381,49 +2600,49 @@
         <v>1</v>
       </c>
       <c r="Y8" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="Z8" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="AA8" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="AB8" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="AC8" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="AD8" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="AE8" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="AF8" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="AG8" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
       <c r="AH8" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="AI8" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="AJ8" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="AK8" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="AL8" t="s">
-        <v>79</v>
+        <v>187</v>
       </c>
       <c r="AM8" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="AN8" t="s">
         <v>73</v>
@@ -2432,7 +2651,7 @@
         <v>0</v>
       </c>
       <c r="AP8">
-        <v>100</v>
+        <v>240</v>
       </c>
       <c r="AQ8" t="s">
         <v>81</v>
@@ -2441,72 +2660,93 @@
         <v>104</v>
       </c>
       <c r="AT8" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="AU8" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="AV8" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="AW8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX8">
-        <v>150</v>
+        <v>165</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>192</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>193</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>194</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:62">
       <c r="A9">
-        <v>43214.54027777778</v>
+        <v>43214.48473379629</v>
       </c>
       <c r="B9">
-        <v>43214.54444444444</v>
+        <v>43214.48878472222</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>43214.54444444444</v>
+        <v>43214.4887962963</v>
       </c>
       <c r="I9" t="s">
-        <v>211</v>
+        <v>196</v>
+      </c>
+      <c r="J9" t="s">
+        <v>197</v>
+      </c>
+      <c r="K9" t="s">
+        <v>198</v>
+      </c>
+      <c r="L9" t="s">
+        <v>199</v>
       </c>
       <c r="N9">
-        <v>45.73539734</v>
+        <v>44.036407470703</v>
       </c>
       <c r="O9">
-        <v>-118.797699</v>
+        <v>-123.05470275879</v>
       </c>
       <c r="P9" t="s">
-        <v>212</v>
+        <v>67</v>
       </c>
       <c r="Q9" t="s">
         <v>68</v>
       </c>
       <c r="R9" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="S9" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="T9" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="U9">
-        <v>97868</v>
+        <v>97426</v>
       </c>
       <c r="V9" t="s">
         <v>72</v>
@@ -2518,49 +2758,49 @@
         <v>1</v>
       </c>
       <c r="Y9" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="Z9" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="AA9" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AB9" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="AC9" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="AD9" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="AE9" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AF9" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="AG9" t="s">
         <v>75</v>
       </c>
       <c r="AH9" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="AI9" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="AJ9" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="AK9" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="AL9" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="AM9" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="AN9" t="s">
         <v>73</v>
@@ -2569,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="AP9">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="AQ9" t="s">
         <v>81</v>
@@ -2578,10 +2818,10 @@
         <v>104</v>
       </c>
       <c r="AT9" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="AU9" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="AV9" t="s">
         <v>107</v>
@@ -2590,69 +2830,60 @@
         <v>73</v>
       </c>
       <c r="AX9">
-        <v>248</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:62">
       <c r="A10">
-        <v>43214.54861111111</v>
+        <v>43214.54048611111</v>
       </c>
       <c r="B10">
-        <v>43214.55555555555</v>
+        <v>43214.54505787037</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="E10">
         <v>100</v>
       </c>
       <c r="F10">
-        <v>646</v>
+        <v>394</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>43214.55555555555</v>
+        <v>43214.54505787037</v>
       </c>
       <c r="I10" t="s">
-        <v>228</v>
-      </c>
-      <c r="J10" t="s">
-        <v>229</v>
-      </c>
-      <c r="K10" t="s">
-        <v>230</v>
-      </c>
-      <c r="L10" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="N10">
-        <v>45.62319946</v>
+        <v>45.735397338867</v>
       </c>
       <c r="O10">
-        <v>-123.9100952</v>
+        <v>-118.79769897461</v>
       </c>
       <c r="P10" t="s">
-        <v>67</v>
+        <v>212</v>
       </c>
       <c r="Q10" t="s">
         <v>68</v>
       </c>
       <c r="R10" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="S10" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="T10" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="U10">
-        <v>97136</v>
+        <v>97868</v>
       </c>
       <c r="V10" t="s">
         <v>72</v>
@@ -2664,49 +2895,49 @@
         <v>1</v>
       </c>
       <c r="Y10" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="Z10" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="AA10" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="AB10" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="AC10" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="AD10" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="AE10" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="AF10" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="AG10" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="AH10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="AI10" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="AJ10" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="AK10" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="AL10" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="AM10" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="AN10" t="s">
         <v>73</v>
@@ -2715,19 +2946,19 @@
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="AQ10" t="s">
         <v>81</v>
       </c>
       <c r="AR10" t="s">
-        <v>245</v>
+        <v>104</v>
       </c>
       <c r="AT10" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="AU10" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="AV10" t="s">
         <v>107</v>
@@ -2736,51 +2967,51 @@
         <v>73</v>
       </c>
       <c r="AX10">
-        <v>300</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:62">
       <c r="A11">
-        <v>43214.55138888889</v>
+        <v>43214.54861111111</v>
       </c>
       <c r="B11">
-        <v>43214.55694444444</v>
+        <v>43214.55609953704</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="E11">
         <v>100</v>
       </c>
       <c r="F11">
-        <v>457</v>
+        <v>646</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>43214.55694444444</v>
+        <v>43214.55609953704</v>
       </c>
       <c r="I11" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="J11" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="K11" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="L11" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="N11">
-        <v>44.36749268</v>
+        <v>45.623199462891</v>
       </c>
       <c r="O11">
-        <v>-118.8083954</v>
+        <v>-123.91009521484</v>
       </c>
       <c r="P11" t="s">
         <v>67</v>
@@ -2789,16 +3020,16 @@
         <v>68</v>
       </c>
       <c r="R11" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="S11" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="T11" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="U11">
-        <v>97906</v>
+        <v>97136</v>
       </c>
       <c r="V11" t="s">
         <v>72</v>
@@ -2810,138 +3041,141 @@
         <v>1</v>
       </c>
       <c r="Y11" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="Z11" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="AA11" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="AB11" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="AC11" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="AD11" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="AE11" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF11">
-        <v>5413582473</v>
+        <v>231</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>239</v>
       </c>
       <c r="AG11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>241</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>242</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>239</v>
+      </c>
+      <c r="AL11" t="s">
         <v>243</v>
       </c>
-      <c r="AH11" t="s">
-        <v>260</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>261</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>262</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>259</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>263</v>
-      </c>
       <c r="AM11" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="AN11" t="s">
         <v>73</v>
       </c>
       <c r="AO11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AP11">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AQ11" t="s">
         <v>81</v>
       </c>
       <c r="AR11" t="s">
-        <v>104</v>
+        <v>245</v>
       </c>
       <c r="AT11" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="AU11" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="AV11" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="AW11" t="s">
-        <v>165</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>267</v>
-      </c>
-      <c r="BA11" t="s">
-        <v>268</v>
-      </c>
-      <c r="BJ11" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AX11">
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:62">
       <c r="A12">
-        <v>43214.53263888889</v>
+        <v>43214.55177083334</v>
       </c>
       <c r="B12">
-        <v>43214.5875</v>
+        <v>43214.55707175926</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="E12">
         <v>100</v>
       </c>
       <c r="F12">
-        <v>4737</v>
+        <v>457</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>43214.5875</v>
+        <v>43214.55707175926</v>
       </c>
       <c r="I12" t="s">
-        <v>270</v>
+        <v>249</v>
+      </c>
+      <c r="J12" t="s">
+        <v>250</v>
+      </c>
+      <c r="K12" t="s">
+        <v>251</v>
+      </c>
+      <c r="L12" t="s">
+        <v>252</v>
       </c>
       <c r="N12">
-        <v>44.03640747</v>
+        <v>44.367492675781</v>
       </c>
       <c r="O12">
-        <v>-123.0547028</v>
+        <v>-118.80839538574</v>
       </c>
       <c r="P12" t="s">
-        <v>212</v>
+        <v>67</v>
       </c>
       <c r="Q12" t="s">
         <v>68</v>
       </c>
       <c r="R12" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="S12" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="T12" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="U12">
-        <v>97455</v>
+        <v>97906</v>
       </c>
       <c r="V12" t="s">
         <v>72</v>
@@ -2953,58 +3187,58 @@
         <v>1</v>
       </c>
       <c r="Y12" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="Z12" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="AA12" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="AB12" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="AC12" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
       <c r="AD12" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="AE12" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>281</v>
+        <v>252</v>
+      </c>
+      <c r="AF12">
+        <v>5413582473</v>
       </c>
       <c r="AG12" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="AH12" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="AI12" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="AJ12" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="AK12" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="AL12" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="AM12" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="AN12" t="s">
         <v>73</v>
       </c>
       <c r="AO12">
+        <v>8</v>
+      </c>
+      <c r="AP12">
         <v>0</v>
-      </c>
-      <c r="AP12">
-        <v>78</v>
       </c>
       <c r="AQ12" t="s">
         <v>81</v>
@@ -3013,19 +3247,1180 @@
         <v>104</v>
       </c>
       <c r="AT12" t="s">
+        <v>265</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>266</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>267</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>268</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62">
+      <c r="A13">
+        <v>43214.53298611111</v>
+      </c>
+      <c r="B13">
+        <v>43214.58782407407</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>269</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>4737</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>43214.58783564815</v>
+      </c>
+      <c r="I13" t="s">
+        <v>270</v>
+      </c>
+      <c r="N13">
+        <v>44.036407470703</v>
+      </c>
+      <c r="O13">
+        <v>-123.05470275879</v>
+      </c>
+      <c r="P13" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>68</v>
+      </c>
+      <c r="R13" t="s">
+        <v>271</v>
+      </c>
+      <c r="S13" t="s">
+        <v>272</v>
+      </c>
+      <c r="T13" t="s">
+        <v>273</v>
+      </c>
+      <c r="U13">
+        <v>97455</v>
+      </c>
+      <c r="V13" t="s">
+        <v>72</v>
+      </c>
+      <c r="W13" t="s">
+        <v>73</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>275</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>276</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>277</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>278</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>279</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>284</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>286</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>287</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>78</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT13" t="s">
         <v>208</v>
       </c>
-      <c r="AU12" t="s">
+      <c r="AU13" t="s">
         <v>288</v>
       </c>
-      <c r="AV12" t="s">
+      <c r="AV13" t="s">
         <v>107</v>
       </c>
-      <c r="AW12" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX12">
+      <c r="AW13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX13">
         <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62">
+      <c r="A14">
+        <v>43215.40797453704</v>
+      </c>
+      <c r="B14">
+        <v>43215.41537037037</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>289</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>639</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>43215.41538194445</v>
+      </c>
+      <c r="I14" t="s">
+        <v>290</v>
+      </c>
+      <c r="J14" t="s">
+        <v>291</v>
+      </c>
+      <c r="K14" t="s">
+        <v>204</v>
+      </c>
+      <c r="L14" t="s">
+        <v>292</v>
+      </c>
+      <c r="N14">
+        <v>44.106597900391</v>
+      </c>
+      <c r="O14">
+        <v>-120.6641998291</v>
+      </c>
+      <c r="P14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14" t="s">
+        <v>293</v>
+      </c>
+      <c r="S14" t="s">
+        <v>294</v>
+      </c>
+      <c r="T14" t="s">
+        <v>295</v>
+      </c>
+      <c r="U14">
+        <v>97754</v>
+      </c>
+      <c r="V14" t="s">
+        <v>72</v>
+      </c>
+      <c r="W14" t="s">
+        <v>73</v>
+      </c>
+      <c r="X14">
+        <v>4</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>297</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>298</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>292</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>300</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>301</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>302</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>303</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>304</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>306</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>307</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>207</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>308</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>164</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>309</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX14">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62">
+      <c r="AM15" t="s">
+        <v>310</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>2</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>308</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>164</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>309</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX15">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62">
+      <c r="AM16" t="s">
+        <v>311</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>2</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>308</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>164</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:61">
+      <c r="A17">
+        <v>43215.50027777778</v>
+      </c>
+      <c r="B17">
+        <v>43215.52997685185</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>312</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>2565</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>43215.52998842593</v>
+      </c>
+      <c r="I17" t="s">
+        <v>313</v>
+      </c>
+      <c r="J17" t="s">
+        <v>314</v>
+      </c>
+      <c r="K17" t="s">
+        <v>315</v>
+      </c>
+      <c r="L17" t="s">
+        <v>316</v>
+      </c>
+      <c r="N17">
+        <v>44.08610534668</v>
+      </c>
+      <c r="O17">
+        <v>-117.01879882812</v>
+      </c>
+      <c r="P17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>68</v>
+      </c>
+      <c r="R17" t="s">
+        <v>317</v>
+      </c>
+      <c r="S17" t="s">
+        <v>318</v>
+      </c>
+      <c r="T17" t="s">
+        <v>319</v>
+      </c>
+      <c r="U17">
+        <v>97901</v>
+      </c>
+      <c r="V17" t="s">
+        <v>72</v>
+      </c>
+      <c r="W17" t="s">
+        <v>73</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>321</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB17">
+        <v>5413722335</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>323</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>321</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>322</v>
+      </c>
+      <c r="AF17">
+        <v>5413722335</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>315</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>314</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>324</v>
+      </c>
+      <c r="AK17">
+        <v>5413722335</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>325</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>326</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>27</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>327</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>328</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>328</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>329</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX17">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:61">
+      <c r="A18">
+        <v>43215.52734953703</v>
+      </c>
+      <c r="B18">
+        <v>43215.55709490741</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>2570</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>43215.55709490741</v>
+      </c>
+      <c r="I18" t="s">
+        <v>331</v>
+      </c>
+      <c r="J18" t="s">
+        <v>332</v>
+      </c>
+      <c r="K18" t="s">
+        <v>333</v>
+      </c>
+      <c r="L18" t="s">
+        <v>334</v>
+      </c>
+      <c r="N18">
+        <v>45.153396606445</v>
+      </c>
+      <c r="O18">
+        <v>-117.77230072021</v>
+      </c>
+      <c r="P18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>68</v>
+      </c>
+      <c r="R18" t="s">
+        <v>335</v>
+      </c>
+      <c r="S18" t="s">
+        <v>336</v>
+      </c>
+      <c r="T18" t="s">
+        <v>337</v>
+      </c>
+      <c r="U18">
+        <v>97841</v>
+      </c>
+      <c r="V18" t="s">
+        <v>72</v>
+      </c>
+      <c r="W18" t="s">
+        <v>73</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>333</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB18">
+        <v>5415345331</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>334</v>
+      </c>
+      <c r="AF18">
+        <v>5415345331</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>338</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>339</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>340</v>
+      </c>
+      <c r="AK18">
+        <v>5415345331</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>341</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>342</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>25</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX18">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:61">
+      <c r="A19">
+        <v>43215.59530092592</v>
+      </c>
+      <c r="B19">
+        <v>43215.6015625</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>343</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>541</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>43215.6015625</v>
+      </c>
+      <c r="I19" t="s">
+        <v>344</v>
+      </c>
+      <c r="N19">
+        <v>44.841903686523</v>
+      </c>
+      <c r="O19">
+        <v>-123.08860015869</v>
+      </c>
+      <c r="P19" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>68</v>
+      </c>
+      <c r="S19" t="s">
+        <v>345</v>
+      </c>
+      <c r="T19" t="s">
+        <v>346</v>
+      </c>
+      <c r="U19">
+        <v>97321</v>
+      </c>
+      <c r="V19" t="s">
+        <v>72</v>
+      </c>
+      <c r="W19" t="s">
+        <v>73</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>345</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>347</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>348</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>347</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>349</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>350</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>345</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>349</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>351</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO19">
+        <v>12</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:61">
+      <c r="A20">
+        <v>43214.41291666667</v>
+      </c>
+      <c r="B20">
+        <v>43216.51513888889</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>353</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>181631</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>43216.51513888889</v>
+      </c>
+      <c r="I20" t="s">
+        <v>354</v>
+      </c>
+      <c r="J20" t="s">
+        <v>355</v>
+      </c>
+      <c r="K20" t="s">
+        <v>216</v>
+      </c>
+      <c r="L20" t="s">
+        <v>356</v>
+      </c>
+      <c r="N20">
+        <v>43.597900390625</v>
+      </c>
+      <c r="O20">
+        <v>-118.89579772949</v>
+      </c>
+      <c r="P20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20" t="s">
+        <v>357</v>
+      </c>
+      <c r="S20" t="s">
+        <v>358</v>
+      </c>
+      <c r="T20" t="s">
+        <v>359</v>
+      </c>
+      <c r="U20">
+        <v>97720</v>
+      </c>
+      <c r="V20" t="s">
+        <v>72</v>
+      </c>
+      <c r="W20" t="s">
+        <v>73</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>360</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>355</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>356</v>
+      </c>
+      <c r="AB20">
+        <v>5415736811</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>361</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>362</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>363</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>364</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>365</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>366</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>367</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>368</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>364</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>263</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>369</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>65</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>370</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>371</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>372</v>
+      </c>
+      <c r="AV20" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX20">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:61">
+      <c r="A21">
+        <v>43216.66710648148</v>
+      </c>
+      <c r="B21">
+        <v>43216.69556712963</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>373</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>2459</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>43216.6955787037</v>
+      </c>
+      <c r="I21" t="s">
+        <v>374</v>
+      </c>
+      <c r="J21" t="s">
+        <v>375</v>
+      </c>
+      <c r="K21" t="s">
+        <v>376</v>
+      </c>
+      <c r="L21" t="s">
+        <v>377</v>
+      </c>
+      <c r="N21">
+        <v>45.457305908203</v>
+      </c>
+      <c r="O21">
+        <v>-122.79919433594</v>
+      </c>
+      <c r="P21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>68</v>
+      </c>
+      <c r="R21" t="s">
+        <v>378</v>
+      </c>
+      <c r="S21" t="s">
+        <v>379</v>
+      </c>
+      <c r="T21" t="s">
+        <v>380</v>
+      </c>
+      <c r="U21">
+        <v>97138</v>
+      </c>
+      <c r="V21" t="s">
+        <v>72</v>
+      </c>
+      <c r="W21" t="s">
+        <v>73</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>382</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>383</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>384</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>381</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>382</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>383</v>
+      </c>
+      <c r="AF21">
+        <v>5037552451</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>376</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>375</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>385</v>
+      </c>
+      <c r="AK21">
+        <v>5037552451</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>386</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>13</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>245</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>387</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>388</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>389</v>
+      </c>
+      <c r="BA21" t="s">
+        <v>167</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD21">
+        <v>239</v>
+      </c>
+      <c r="BE21">
+        <v>20</v>
+      </c>
+      <c r="BF21">
+        <v>45</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="AM1:BJ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="39:62">
+      <c r="AM1" t="s">
+        <v>390</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>391</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>392</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>393</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>394</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>396</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>397</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>398</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>399</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>400</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>401</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>402</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>403</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>404</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>405</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>406</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>407</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>408</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>409</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>410</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>411</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>412</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code to print on a new line although I have a blank line at the end
</commit_message>
<xml_diff>
--- a/SummerWork-2/OUTPUT.xlsx
+++ b/SummerWork-2/OUTPUT.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="392">
   <si>
     <t>Start Date</t>
   </si>
@@ -522,6 +522,9 @@
     <t>Request Additional Funds beyond the threshold from Measure 99 Outdoor School Funds within this application</t>
   </si>
   <si>
+    <t>Warm Springs K-8 Academy</t>
+  </si>
+  <si>
     <t>198.237.133.2</t>
   </si>
   <si>
@@ -954,6 +957,9 @@
     <t>Brothers Elementary School</t>
   </si>
   <si>
+    <t>Powell Butte Community Charter School</t>
+  </si>
+  <si>
     <t>198.237.103.59</t>
   </si>
   <si>
@@ -1186,79 +1192,6 @@
   </si>
   <si>
     <t>Traveling Long Distance to Facility</t>
-  </si>
-  <si>
-    <t>2 - School Number:  [CurrentLoopNumber]Please Provide the Name:</t>
-  </si>
-  <si>
-    <t>2 - Has this school participated in any outdoor school programs before the 18-19 fiscal year?</t>
-  </si>
-  <si>
-    <t>Number of students attending Outdoor School in each grade.  Add 0 if there are no students attending in one or other grade. - 2 - 5th Grade</t>
-  </si>
-  <si>
-    <t>Number of students attending Outdoor School in each grade.  Add 0 if there are no students attending in one or other grade. - 2 - 6th Grade</t>
-  </si>
-  <si>
-    <t>2 - I certify that the student count listed above does not include students who previously attended outdoor school using Measure 99 Outdoor School Funds in 2017-2018.</t>
-  </si>
-  <si>
-    <t>Name of Outdoor School Provider for [QID9-ChoiceTextEntryValue]: - 2 - Name of Outdoor School Provider for [QID9-ChoiceTextEntryValue]: - Selected Choice</t>
-  </si>
-  <si>
-    <t>Name of Outdoor School Provider for [QID9-ChoiceTextEntryValue]: - 2 - Other - Text</t>
-  </si>
-  <si>
-    <t>Location of Camp/Facility - 2 - Name of Camp or Facility</t>
-  </si>
-  <si>
-    <t>Location of Camp/Facility - 2 - Closest City to Camp or Facility</t>
-  </si>
-  <si>
-    <t>2 - Length of Program</t>
-  </si>
-  <si>
-    <t>2 - Based on the table above, will the anticipated threshold amount per student for your program length be adequate for  [QID9-ChoiceTextEntryValue]?</t>
-  </si>
-  <si>
-    <t>2 - If threshold is enough, what do you anticipate the costs for [QID9-ChoiceTextEntryValue] being per student (please round up to whole dollar)?</t>
-  </si>
-  <si>
-    <t>Reason additional funds are needed (Check all that apply): - 2 - Reason additional funds are needed (Check all that apply): - Selected Choice</t>
-  </si>
-  <si>
-    <t>Reason additional funds are needed (Check all that apply): - 2 - Other - Text</t>
-  </si>
-  <si>
-    <t>Additional funding plans (Check all that apply): - 2 - Additional funding plans (Check all that apply): - Selected Choice</t>
-  </si>
-  <si>
-    <t>Additional funding plans (Check all that apply): - 2 - Other - Text</t>
-  </si>
-  <si>
-    <t>2 - I have reviewed the budget categories &amp; definitions and am prepared to provide a detailed budget to request for additional costs.</t>
-  </si>
-  <si>
-    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Outdoor School Provider Fees</t>
-  </si>
-  <si>
-    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Transportation</t>
-  </si>
-  <si>
-    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Personnel/Stipends</t>
-  </si>
-  <si>
-    <t>Please complete the following table for the total funds PER STUDENT  for [QID9-ChoiceTextEntryValue] for which you are requesting funding in this application.  The total requested amount per student will display on the next page. - 2 - Program Costs incurred by District or School without administration costs</t>
-  </si>
-  <si>
-    <t>2 - Any details you would like the reviewers to consider regarding your request.</t>
-  </si>
-  <si>
-    <t>2 - [QID9-ChoiceTextEntryValue] is asking a total of  $[QID40-TotalSum] per student based on the slide table in page before.  I understand these funds are not guaranteed until I receive my Work Order and funding approval.
-While we cannot assign actual funding amounts prior to receipt of all 2018-2019 applications, the information you provided will be presented to the review team.  The review team will consider your request in conjunction with fund availability and statewide needs.  OSU will attempt to cover all or a portion of the requested funding.</t>
-  </si>
-  <si>
-    <t>2 - Although my costs are higher than the Measure 99 funding threshold, I will be using other options to fund the difference.  Therefore my application is requesting funds based on the threshold for my length of program.</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1523,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BJ21"/>
+  <dimension ref="A1:BJ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2529,206 +2462,98 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:62">
-      <c r="A8">
-        <v>43213.67719907407</v>
-      </c>
-      <c r="B8">
-        <v>43214.42510416666</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="7" spans="1:62">
+      <c r="AM7" t="s">
         <v>168</v>
       </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>64618</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>43214.42511574074</v>
-      </c>
-      <c r="I8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J8" t="s">
-        <v>170</v>
-      </c>
-      <c r="K8" t="s">
-        <v>171</v>
-      </c>
-      <c r="L8" t="s">
-        <v>172</v>
-      </c>
-      <c r="N8">
-        <v>42.538604736328</v>
-      </c>
-      <c r="O8">
-        <v>-123.3478012085</v>
-      </c>
-      <c r="P8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>68</v>
-      </c>
-      <c r="R8" t="s">
-        <v>173</v>
-      </c>
-      <c r="S8" t="s">
-        <v>174</v>
-      </c>
-      <c r="T8" t="s">
-        <v>175</v>
-      </c>
-      <c r="U8">
-        <v>97526</v>
-      </c>
-      <c r="V8" t="s">
+      <c r="AN7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO7">
+        <v>66</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>167</v>
+      </c>
+      <c r="BC7" t="s">
         <v>72</v>
       </c>
-      <c r="W8" t="s">
-        <v>73</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC8" t="s">
+      <c r="BD7">
         <v>180</v>
       </c>
-      <c r="AD8" t="s">
-        <v>181</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>172</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>183</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>184</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>185</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>179</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>187</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>188</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO8">
-        <v>0</v>
-      </c>
-      <c r="AP8">
-        <v>240</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>189</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>190</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>165</v>
-      </c>
-      <c r="AY8" t="s">
-        <v>191</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>192</v>
-      </c>
-      <c r="BA8" t="s">
-        <v>193</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>194</v>
-      </c>
-      <c r="BJ8" t="s">
+      <c r="BE7">
+        <v>10</v>
+      </c>
+      <c r="BI7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:62">
       <c r="A9">
-        <v>43214.48473379629</v>
+        <v>43213.67719907407</v>
       </c>
       <c r="B9">
-        <v>43214.48878472222</v>
+        <v>43214.42510416666</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>350</v>
+        <v>64618</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>43214.4887962963</v>
+        <v>43214.42511574074</v>
       </c>
       <c r="I9" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="J9" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="K9" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="L9" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="N9">
-        <v>44.036407470703</v>
+        <v>42.538604736328</v>
       </c>
       <c r="O9">
-        <v>-123.05470275879</v>
+        <v>-123.3478012085</v>
       </c>
       <c r="P9" t="s">
         <v>67</v>
@@ -2737,16 +2562,16 @@
         <v>68</v>
       </c>
       <c r="R9" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="S9" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="T9" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="U9">
-        <v>97426</v>
+        <v>97526</v>
       </c>
       <c r="V9" t="s">
         <v>72</v>
@@ -2758,49 +2583,49 @@
         <v>1</v>
       </c>
       <c r="Y9" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="Z9" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="AA9" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="AB9" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="AC9" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="AD9" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="AE9" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="AF9" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="AG9" t="s">
-        <v>75</v>
+        <v>184</v>
       </c>
       <c r="AH9" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="AI9" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="AJ9" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="AK9" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="AL9" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
       <c r="AM9" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="AN9" t="s">
         <v>73</v>
@@ -2809,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="AP9">
-        <v>100</v>
+        <v>240</v>
       </c>
       <c r="AQ9" t="s">
         <v>81</v>
@@ -2818,72 +2643,93 @@
         <v>104</v>
       </c>
       <c r="AT9" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="AU9" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="AV9" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="AW9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX9">
-        <v>150</v>
+        <v>165</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>192</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>193</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>194</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>195</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:62">
       <c r="A10">
-        <v>43214.54048611111</v>
+        <v>43214.48473379629</v>
       </c>
       <c r="B10">
-        <v>43214.54505787037</v>
+        <v>43214.48878472222</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="E10">
         <v>100</v>
       </c>
       <c r="F10">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>43214.54505787037</v>
+        <v>43214.4887962963</v>
       </c>
       <c r="I10" t="s">
-        <v>211</v>
+        <v>197</v>
+      </c>
+      <c r="J10" t="s">
+        <v>198</v>
+      </c>
+      <c r="K10" t="s">
+        <v>199</v>
+      </c>
+      <c r="L10" t="s">
+        <v>200</v>
       </c>
       <c r="N10">
-        <v>45.735397338867</v>
+        <v>44.036407470703</v>
       </c>
       <c r="O10">
-        <v>-118.79769897461</v>
+        <v>-123.05470275879</v>
       </c>
       <c r="P10" t="s">
-        <v>212</v>
+        <v>67</v>
       </c>
       <c r="Q10" t="s">
         <v>68</v>
       </c>
       <c r="R10" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="S10" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="T10" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="U10">
-        <v>97868</v>
+        <v>97426</v>
       </c>
       <c r="V10" t="s">
         <v>72</v>
@@ -2895,49 +2741,49 @@
         <v>1</v>
       </c>
       <c r="Y10" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="Z10" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AA10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="AB10" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="AC10" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="AD10" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AE10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="AF10" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="AG10" t="s">
         <v>75</v>
       </c>
       <c r="AH10" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="AI10" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="AJ10" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="AK10" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="AL10" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="AM10" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="AN10" t="s">
         <v>73</v>
@@ -2946,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="AQ10" t="s">
         <v>81</v>
@@ -2955,10 +2801,10 @@
         <v>104</v>
       </c>
       <c r="AT10" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="AU10" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="AV10" t="s">
         <v>107</v>
@@ -2967,69 +2813,60 @@
         <v>73</v>
       </c>
       <c r="AX10">
-        <v>248</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:62">
       <c r="A11">
-        <v>43214.54861111111</v>
+        <v>43214.54048611111</v>
       </c>
       <c r="B11">
-        <v>43214.55609953704</v>
+        <v>43214.54505787037</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="E11">
         <v>100</v>
       </c>
       <c r="F11">
-        <v>646</v>
+        <v>394</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>43214.55609953704</v>
+        <v>43214.54505787037</v>
       </c>
       <c r="I11" t="s">
-        <v>228</v>
-      </c>
-      <c r="J11" t="s">
-        <v>229</v>
-      </c>
-      <c r="K11" t="s">
-        <v>230</v>
-      </c>
-      <c r="L11" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="N11">
-        <v>45.623199462891</v>
+        <v>45.735397338867</v>
       </c>
       <c r="O11">
-        <v>-123.91009521484</v>
+        <v>-118.79769897461</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>213</v>
       </c>
       <c r="Q11" t="s">
         <v>68</v>
       </c>
       <c r="R11" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="S11" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="T11" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="U11">
-        <v>97136</v>
+        <v>97868</v>
       </c>
       <c r="V11" t="s">
         <v>72</v>
@@ -3041,49 +2878,49 @@
         <v>1</v>
       </c>
       <c r="Y11" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="Z11" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="AA11" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="AB11" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="AC11" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="AD11" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="AE11" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="AF11" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="AG11" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="AH11" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="AI11" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="AJ11" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="AK11" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="AL11" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="AM11" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="AN11" t="s">
         <v>73</v>
@@ -3092,19 +2929,19 @@
         <v>0</v>
       </c>
       <c r="AP11">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="AQ11" t="s">
         <v>81</v>
       </c>
       <c r="AR11" t="s">
-        <v>245</v>
+        <v>104</v>
       </c>
       <c r="AT11" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="AU11" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="AV11" t="s">
         <v>107</v>
@@ -3113,51 +2950,51 @@
         <v>73</v>
       </c>
       <c r="AX11">
-        <v>300</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:62">
       <c r="A12">
-        <v>43214.55177083334</v>
+        <v>43214.54861111111</v>
       </c>
       <c r="B12">
-        <v>43214.55707175926</v>
+        <v>43214.55609953704</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="E12">
         <v>100</v>
       </c>
       <c r="F12">
-        <v>457</v>
+        <v>646</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>43214.55707175926</v>
+        <v>43214.55609953704</v>
       </c>
       <c r="I12" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="J12" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="K12" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="L12" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="N12">
-        <v>44.367492675781</v>
+        <v>45.623199462891</v>
       </c>
       <c r="O12">
-        <v>-118.80839538574</v>
+        <v>-123.91009521484</v>
       </c>
       <c r="P12" t="s">
         <v>67</v>
@@ -3166,16 +3003,16 @@
         <v>68</v>
       </c>
       <c r="R12" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="S12" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="T12" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="U12">
-        <v>97906</v>
+        <v>97136</v>
       </c>
       <c r="V12" t="s">
         <v>72</v>
@@ -3187,138 +3024,141 @@
         <v>1</v>
       </c>
       <c r="Y12" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="Z12" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="AA12" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="AB12" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="AC12" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="AD12" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="AE12" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF12">
-        <v>5413582473</v>
+        <v>232</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>240</v>
       </c>
       <c r="AG12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>242</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>243</v>
       </c>
-      <c r="AH12" t="s">
-        <v>260</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>261</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>262</v>
-      </c>
       <c r="AK12" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="AL12" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="AM12" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="AN12" t="s">
         <v>73</v>
       </c>
       <c r="AO12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AP12">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AQ12" t="s">
         <v>81</v>
       </c>
       <c r="AR12" t="s">
-        <v>104</v>
+        <v>246</v>
       </c>
       <c r="AT12" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="AU12" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="AV12" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="AW12" t="s">
-        <v>165</v>
-      </c>
-      <c r="AY12" t="s">
-        <v>267</v>
-      </c>
-      <c r="BA12" t="s">
-        <v>268</v>
-      </c>
-      <c r="BJ12" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AX12">
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:62">
       <c r="A13">
-        <v>43214.53298611111</v>
+        <v>43214.55177083334</v>
       </c>
       <c r="B13">
-        <v>43214.58782407407</v>
+        <v>43214.55707175926</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="E13">
         <v>100</v>
       </c>
       <c r="F13">
-        <v>4737</v>
+        <v>457</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>43214.58783564815</v>
+        <v>43214.55707175926</v>
       </c>
       <c r="I13" t="s">
-        <v>270</v>
+        <v>250</v>
+      </c>
+      <c r="J13" t="s">
+        <v>251</v>
+      </c>
+      <c r="K13" t="s">
+        <v>252</v>
+      </c>
+      <c r="L13" t="s">
+        <v>253</v>
       </c>
       <c r="N13">
-        <v>44.036407470703</v>
+        <v>44.367492675781</v>
       </c>
       <c r="O13">
-        <v>-123.05470275879</v>
+        <v>-118.80839538574</v>
       </c>
       <c r="P13" t="s">
-        <v>212</v>
+        <v>67</v>
       </c>
       <c r="Q13" t="s">
         <v>68</v>
       </c>
       <c r="R13" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="S13" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="T13" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="U13">
-        <v>97455</v>
+        <v>97906</v>
       </c>
       <c r="V13" t="s">
         <v>72</v>
@@ -3330,58 +3170,58 @@
         <v>1</v>
       </c>
       <c r="Y13" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="Z13" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="AA13" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="AB13" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="AC13" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="AD13" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="AE13" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>281</v>
+        <v>253</v>
+      </c>
+      <c r="AF13">
+        <v>5413582473</v>
       </c>
       <c r="AG13" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="AH13" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="AI13" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="AJ13" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
       <c r="AK13" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="AL13" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="AM13" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="AN13" t="s">
         <v>73</v>
       </c>
       <c r="AO13">
+        <v>8</v>
+      </c>
+      <c r="AP13">
         <v>0</v>
-      </c>
-      <c r="AP13">
-        <v>78</v>
       </c>
       <c r="AQ13" t="s">
         <v>81</v>
@@ -3390,81 +3230,78 @@
         <v>104</v>
       </c>
       <c r="AT13" t="s">
-        <v>208</v>
+        <v>266</v>
       </c>
       <c r="AU13" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="AV13" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="AW13" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX13">
-        <v>248</v>
+        <v>165</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>268</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>269</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:62">
       <c r="A14">
-        <v>43215.40797453704</v>
+        <v>43214.53298611111</v>
       </c>
       <c r="B14">
-        <v>43215.41537037037</v>
+        <v>43214.58782407407</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="E14">
         <v>100</v>
       </c>
       <c r="F14">
-        <v>639</v>
+        <v>4737</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>43215.41538194445</v>
+        <v>43214.58783564815</v>
       </c>
       <c r="I14" t="s">
-        <v>290</v>
-      </c>
-      <c r="J14" t="s">
-        <v>291</v>
-      </c>
-      <c r="K14" t="s">
-        <v>204</v>
-      </c>
-      <c r="L14" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="N14">
-        <v>44.106597900391</v>
+        <v>44.036407470703</v>
       </c>
       <c r="O14">
-        <v>-120.6641998291</v>
+        <v>-123.05470275879</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>213</v>
       </c>
       <c r="Q14" t="s">
         <v>68</v>
       </c>
       <c r="R14" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="S14" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="T14" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="U14">
-        <v>97754</v>
+        <v>97455</v>
       </c>
       <c r="V14" t="s">
         <v>72</v>
@@ -3473,52 +3310,52 @@
         <v>73</v>
       </c>
       <c r="X14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y14" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="Z14" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="AA14" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="AB14" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="AC14" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="AD14" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="AE14" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="AF14" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="AG14" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="AH14" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="AI14" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="AJ14" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="AK14" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="AL14" t="s">
-        <v>306</v>
+        <v>79</v>
       </c>
       <c r="AM14" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="AN14" t="s">
         <v>73</v>
@@ -3527,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="AP14">
-        <v>207</v>
+        <v>78</v>
       </c>
       <c r="AQ14" t="s">
         <v>81</v>
@@ -3536,24 +3373,135 @@
         <v>104</v>
       </c>
       <c r="AT14" t="s">
-        <v>308</v>
+        <v>209</v>
       </c>
       <c r="AU14" t="s">
-        <v>164</v>
+        <v>289</v>
       </c>
       <c r="AV14" t="s">
-        <v>309</v>
+        <v>107</v>
       </c>
       <c r="AW14" t="s">
         <v>73</v>
       </c>
       <c r="AX14">
-        <v>304</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:62">
+      <c r="A15">
+        <v>43215.40797453704</v>
+      </c>
+      <c r="B15">
+        <v>43215.41537037037</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>639</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>43215.41538194445</v>
+      </c>
+      <c r="I15" t="s">
+        <v>291</v>
+      </c>
+      <c r="J15" t="s">
+        <v>292</v>
+      </c>
+      <c r="K15" t="s">
+        <v>205</v>
+      </c>
+      <c r="L15" t="s">
+        <v>293</v>
+      </c>
+      <c r="N15">
+        <v>44.106597900391</v>
+      </c>
+      <c r="O15">
+        <v>-120.6641998291</v>
+      </c>
+      <c r="P15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>68</v>
+      </c>
+      <c r="R15" t="s">
+        <v>294</v>
+      </c>
+      <c r="S15" t="s">
+        <v>295</v>
+      </c>
+      <c r="T15" t="s">
+        <v>296</v>
+      </c>
+      <c r="U15">
+        <v>97754</v>
+      </c>
+      <c r="V15" t="s">
+        <v>72</v>
+      </c>
+      <c r="W15" t="s">
+        <v>73</v>
+      </c>
+      <c r="X15">
+        <v>4</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>292</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>293</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>302</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>303</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>304</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>305</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>306</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>307</v>
+      </c>
       <c r="AM15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AN15" t="s">
         <v>73</v>
@@ -3562,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="AP15">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="AQ15" t="s">
         <v>81</v>
@@ -3571,13 +3519,13 @@
         <v>104</v>
       </c>
       <c r="AT15" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AU15" t="s">
         <v>164</v>
       </c>
       <c r="AV15" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AW15" t="s">
         <v>73</v>
@@ -3606,129 +3554,24 @@
         <v>104</v>
       </c>
       <c r="AT16" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AU16" t="s">
         <v>164</v>
       </c>
       <c r="AV16" t="s">
-        <v>309</v>
+        <v>310</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX16">
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:61">
-      <c r="A17">
-        <v>43215.50027777778</v>
-      </c>
-      <c r="B17">
-        <v>43215.52997685185</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="AM17" t="s">
         <v>312</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-      <c r="F17">
-        <v>2565</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>43215.52998842593</v>
-      </c>
-      <c r="I17" t="s">
-        <v>313</v>
-      </c>
-      <c r="J17" t="s">
-        <v>314</v>
-      </c>
-      <c r="K17" t="s">
-        <v>315</v>
-      </c>
-      <c r="L17" t="s">
-        <v>316</v>
-      </c>
-      <c r="N17">
-        <v>44.08610534668</v>
-      </c>
-      <c r="O17">
-        <v>-117.01879882812</v>
-      </c>
-      <c r="P17" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>68</v>
-      </c>
-      <c r="R17" t="s">
-        <v>317</v>
-      </c>
-      <c r="S17" t="s">
-        <v>318</v>
-      </c>
-      <c r="T17" t="s">
-        <v>319</v>
-      </c>
-      <c r="U17">
-        <v>97901</v>
-      </c>
-      <c r="V17" t="s">
-        <v>72</v>
-      </c>
-      <c r="W17" t="s">
-        <v>73</v>
-      </c>
-      <c r="X17">
-        <v>1</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>320</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>321</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>322</v>
-      </c>
-      <c r="AB17">
-        <v>5413722335</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>323</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>321</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>322</v>
-      </c>
-      <c r="AF17">
-        <v>5413722335</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>315</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>314</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>324</v>
-      </c>
-      <c r="AK17">
-        <v>5413722335</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>325</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>326</v>
       </c>
       <c r="AN17" t="s">
         <v>73</v>
@@ -3737,147 +3580,33 @@
         <v>0</v>
       </c>
       <c r="AP17">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="AQ17" t="s">
         <v>81</v>
       </c>
       <c r="AR17" t="s">
-        <v>327</v>
-      </c>
-      <c r="AS17" t="s">
-        <v>328</v>
+        <v>104</v>
       </c>
       <c r="AT17" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="AU17" t="s">
-        <v>329</v>
+        <v>164</v>
       </c>
       <c r="AV17" t="s">
-        <v>107</v>
+        <v>310</v>
       </c>
       <c r="AW17" t="s">
         <v>73</v>
       </c>
       <c r="AX17">
-        <v>248</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:61">
-      <c r="A18">
-        <v>43215.52734953703</v>
-      </c>
-      <c r="B18">
-        <v>43215.55709490741</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>330</v>
-      </c>
-      <c r="E18">
-        <v>100</v>
-      </c>
-      <c r="F18">
-        <v>2570</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>43215.55709490741</v>
-      </c>
-      <c r="I18" t="s">
-        <v>331</v>
-      </c>
-      <c r="J18" t="s">
-        <v>332</v>
-      </c>
-      <c r="K18" t="s">
-        <v>333</v>
-      </c>
-      <c r="L18" t="s">
-        <v>334</v>
-      </c>
-      <c r="N18">
-        <v>45.153396606445</v>
-      </c>
-      <c r="O18">
-        <v>-117.77230072021</v>
-      </c>
-      <c r="P18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>68</v>
-      </c>
-      <c r="R18" t="s">
-        <v>335</v>
-      </c>
-      <c r="S18" t="s">
-        <v>336</v>
-      </c>
-      <c r="T18" t="s">
-        <v>337</v>
-      </c>
-      <c r="U18">
-        <v>97841</v>
-      </c>
-      <c r="V18" t="s">
-        <v>72</v>
-      </c>
-      <c r="W18" t="s">
-        <v>73</v>
-      </c>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>333</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>332</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>334</v>
-      </c>
-      <c r="AB18">
-        <v>5415345331</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>333</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>332</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>334</v>
-      </c>
-      <c r="AF18">
-        <v>5415345331</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>338</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>339</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>340</v>
-      </c>
-      <c r="AK18">
-        <v>5415345331</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>341</v>
-      </c>
       <c r="AM18" t="s">
-        <v>342</v>
+        <v>313</v>
       </c>
       <c r="AN18" t="s">
         <v>73</v>
@@ -3886,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="AP18">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AQ18" t="s">
         <v>81</v>
@@ -3895,179 +3624,63 @@
         <v>104</v>
       </c>
       <c r="AT18" t="s">
-        <v>82</v>
+        <v>309</v>
       </c>
       <c r="AU18" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="AV18" t="s">
-        <v>85</v>
+        <v>310</v>
       </c>
       <c r="AW18" t="s">
         <v>73</v>
       </c>
       <c r="AX18">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:61">
-      <c r="A19">
-        <v>43215.59530092592</v>
-      </c>
-      <c r="B19">
-        <v>43215.6015625</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>343</v>
-      </c>
-      <c r="E19">
-        <v>100</v>
-      </c>
-      <c r="F19">
-        <v>541</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>43215.6015625</v>
-      </c>
-      <c r="I19" t="s">
-        <v>344</v>
-      </c>
-      <c r="N19">
-        <v>44.841903686523</v>
-      </c>
-      <c r="O19">
-        <v>-123.08860015869</v>
-      </c>
-      <c r="P19" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>68</v>
-      </c>
-      <c r="S19" t="s">
-        <v>345</v>
-      </c>
-      <c r="T19" t="s">
-        <v>346</v>
-      </c>
-      <c r="U19">
-        <v>97321</v>
-      </c>
-      <c r="V19" t="s">
-        <v>72</v>
-      </c>
-      <c r="W19" t="s">
-        <v>73</v>
-      </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>345</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>345</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>347</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>348</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>345</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>345</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>347</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>349</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>350</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>345</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>345</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>347</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>349</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>345</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>351</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO19">
-        <v>12</v>
-      </c>
-      <c r="AP19">
-        <v>0</v>
-      </c>
-      <c r="AQ19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:61">
       <c r="A20">
-        <v>43214.41291666667</v>
+        <v>43215.50027777778</v>
       </c>
       <c r="B20">
-        <v>43216.51513888889</v>
+        <v>43215.52997685185</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>353</v>
+        <v>314</v>
       </c>
       <c r="E20">
         <v>100</v>
       </c>
       <c r="F20">
-        <v>181631</v>
+        <v>2565</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>43216.51513888889</v>
+        <v>43215.52998842593</v>
       </c>
       <c r="I20" t="s">
-        <v>354</v>
+        <v>315</v>
       </c>
       <c r="J20" t="s">
-        <v>355</v>
+        <v>316</v>
       </c>
       <c r="K20" t="s">
-        <v>216</v>
+        <v>317</v>
       </c>
       <c r="L20" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
       <c r="N20">
-        <v>43.597900390625</v>
+        <v>44.08610534668</v>
       </c>
       <c r="O20">
-        <v>-118.89579772949</v>
+        <v>-117.01879882812</v>
       </c>
       <c r="P20" t="s">
         <v>67</v>
@@ -4076,16 +3689,16 @@
         <v>68</v>
       </c>
       <c r="R20" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="S20" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
       <c r="T20" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="U20">
-        <v>97720</v>
+        <v>97901</v>
       </c>
       <c r="V20" t="s">
         <v>72</v>
@@ -4097,49 +3710,49 @@
         <v>1</v>
       </c>
       <c r="Y20" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="Z20" t="s">
-        <v>355</v>
+        <v>323</v>
       </c>
       <c r="AA20" t="s">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="AB20">
-        <v>5415736811</v>
+        <v>5413722335</v>
       </c>
       <c r="AC20" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
       <c r="AD20" t="s">
-        <v>362</v>
+        <v>323</v>
       </c>
       <c r="AE20" t="s">
-        <v>363</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>364</v>
+        <v>324</v>
+      </c>
+      <c r="AF20">
+        <v>5413722335</v>
       </c>
       <c r="AG20" t="s">
-        <v>365</v>
+        <v>75</v>
       </c>
       <c r="AH20" t="s">
-        <v>366</v>
+        <v>317</v>
       </c>
       <c r="AI20" t="s">
-        <v>367</v>
+        <v>316</v>
       </c>
       <c r="AJ20" t="s">
-        <v>368</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>364</v>
+        <v>326</v>
+      </c>
+      <c r="AK20">
+        <v>5413722335</v>
       </c>
       <c r="AL20" t="s">
-        <v>263</v>
+        <v>327</v>
       </c>
       <c r="AM20" t="s">
-        <v>369</v>
+        <v>328</v>
       </c>
       <c r="AN20" t="s">
         <v>73</v>
@@ -4148,72 +3761,75 @@
         <v>0</v>
       </c>
       <c r="AP20">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="AQ20" t="s">
         <v>81</v>
       </c>
       <c r="AR20" t="s">
-        <v>370</v>
+        <v>329</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>330</v>
       </c>
       <c r="AT20" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
       <c r="AU20" t="s">
-        <v>372</v>
+        <v>331</v>
       </c>
       <c r="AV20" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="AW20" t="s">
         <v>73</v>
       </c>
       <c r="AX20">
-        <v>195</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:61">
       <c r="A21">
-        <v>43216.66710648148</v>
+        <v>43215.52734953703</v>
       </c>
       <c r="B21">
-        <v>43216.69556712963</v>
+        <v>43215.55709490741</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="E21">
         <v>100</v>
       </c>
       <c r="F21">
-        <v>2459</v>
+        <v>2570</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21">
-        <v>43216.6955787037</v>
+        <v>43215.55709490741</v>
       </c>
       <c r="I21" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="J21" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
       <c r="K21" t="s">
-        <v>376</v>
+        <v>335</v>
       </c>
       <c r="L21" t="s">
-        <v>377</v>
+        <v>336</v>
       </c>
       <c r="N21">
-        <v>45.457305908203</v>
+        <v>45.153396606445</v>
       </c>
       <c r="O21">
-        <v>-122.79919433594</v>
+        <v>-117.77230072021</v>
       </c>
       <c r="P21" t="s">
         <v>67</v>
@@ -4222,16 +3838,16 @@
         <v>68</v>
       </c>
       <c r="R21" t="s">
-        <v>378</v>
+        <v>337</v>
       </c>
       <c r="S21" t="s">
-        <v>379</v>
+        <v>338</v>
       </c>
       <c r="T21" t="s">
-        <v>380</v>
+        <v>339</v>
       </c>
       <c r="U21">
-        <v>97138</v>
+        <v>97841</v>
       </c>
       <c r="V21" t="s">
         <v>72</v>
@@ -4243,49 +3859,49 @@
         <v>1</v>
       </c>
       <c r="Y21" t="s">
-        <v>381</v>
+        <v>335</v>
       </c>
       <c r="Z21" t="s">
-        <v>382</v>
+        <v>334</v>
       </c>
       <c r="AA21" t="s">
-        <v>383</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>384</v>
+        <v>336</v>
+      </c>
+      <c r="AB21">
+        <v>5415345331</v>
       </c>
       <c r="AC21" t="s">
-        <v>381</v>
+        <v>335</v>
       </c>
       <c r="AD21" t="s">
-        <v>382</v>
+        <v>334</v>
       </c>
       <c r="AE21" t="s">
-        <v>383</v>
+        <v>336</v>
       </c>
       <c r="AF21">
-        <v>5037552451</v>
+        <v>5415345331</v>
       </c>
       <c r="AG21" t="s">
         <v>75</v>
       </c>
       <c r="AH21" t="s">
-        <v>376</v>
+        <v>340</v>
       </c>
       <c r="AI21" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="AJ21" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="AK21">
-        <v>5037552451</v>
+        <v>5415345331</v>
       </c>
       <c r="AL21" t="s">
-        <v>79</v>
+        <v>343</v>
       </c>
       <c r="AM21" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
       <c r="AN21" t="s">
         <v>73</v>
@@ -4294,45 +3910,453 @@
         <v>0</v>
       </c>
       <c r="AP21">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="AQ21" t="s">
         <v>81</v>
       </c>
       <c r="AR21" t="s">
-        <v>245</v>
+        <v>104</v>
       </c>
       <c r="AT21" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX21">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:61">
+      <c r="A22">
+        <v>43215.59530092592</v>
+      </c>
+      <c r="B22">
+        <v>43215.6015625</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>345</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>541</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>43215.6015625</v>
+      </c>
+      <c r="I22" t="s">
+        <v>346</v>
+      </c>
+      <c r="N22">
+        <v>44.841903686523</v>
+      </c>
+      <c r="O22">
+        <v>-123.08860015869</v>
+      </c>
+      <c r="P22" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" t="s">
+        <v>347</v>
+      </c>
+      <c r="T22" t="s">
+        <v>348</v>
+      </c>
+      <c r="U22">
+        <v>97321</v>
+      </c>
+      <c r="V22" t="s">
+        <v>72</v>
+      </c>
+      <c r="W22" t="s">
+        <v>73</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>347</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>349</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>349</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>351</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>352</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>349</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>351</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>347</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>353</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO22">
+        <v>12</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:61">
+      <c r="A23">
+        <v>43214.41291666667</v>
+      </c>
+      <c r="B23">
+        <v>43216.51513888889</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>355</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>181631</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>43216.51513888889</v>
+      </c>
+      <c r="I23" t="s">
+        <v>356</v>
+      </c>
+      <c r="J23" t="s">
+        <v>357</v>
+      </c>
+      <c r="K23" t="s">
+        <v>217</v>
+      </c>
+      <c r="L23" t="s">
+        <v>358</v>
+      </c>
+      <c r="N23">
+        <v>43.597900390625</v>
+      </c>
+      <c r="O23">
+        <v>-118.89579772949</v>
+      </c>
+      <c r="P23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>68</v>
+      </c>
+      <c r="R23" t="s">
+        <v>359</v>
+      </c>
+      <c r="S23" t="s">
+        <v>360</v>
+      </c>
+      <c r="T23" t="s">
+        <v>361</v>
+      </c>
+      <c r="U23">
+        <v>97720</v>
+      </c>
+      <c r="V23" t="s">
+        <v>72</v>
+      </c>
+      <c r="W23" t="s">
+        <v>73</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>362</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB23">
+        <v>5415736811</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>363</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>365</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>366</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>367</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>368</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>369</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>370</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>366</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>264</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>371</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>65</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>372</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>373</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>374</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX23">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:61">
+      <c r="A24">
+        <v>43216.66710648148</v>
+      </c>
+      <c r="B24">
+        <v>43216.69556712963</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>375</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>2459</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>43216.6955787037</v>
+      </c>
+      <c r="I24" t="s">
+        <v>376</v>
+      </c>
+      <c r="J24" t="s">
+        <v>377</v>
+      </c>
+      <c r="K24" t="s">
+        <v>378</v>
+      </c>
+      <c r="L24" t="s">
+        <v>379</v>
+      </c>
+      <c r="N24">
+        <v>45.457305908203</v>
+      </c>
+      <c r="O24">
+        <v>-122.79919433594</v>
+      </c>
+      <c r="P24" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>68</v>
+      </c>
+      <c r="R24" t="s">
+        <v>380</v>
+      </c>
+      <c r="S24" t="s">
+        <v>381</v>
+      </c>
+      <c r="T24" t="s">
+        <v>382</v>
+      </c>
+      <c r="U24">
+        <v>97138</v>
+      </c>
+      <c r="V24" t="s">
+        <v>72</v>
+      </c>
+      <c r="W24" t="s">
+        <v>73</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>384</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>385</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>386</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>384</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>385</v>
+      </c>
+      <c r="AF24">
+        <v>5037552451</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>378</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>377</v>
+      </c>
+      <c r="AJ24" t="s">
         <v>387</v>
       </c>
-      <c r="AU21" t="s">
+      <c r="AK24">
+        <v>5037552451</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM24" t="s">
         <v>388</v>
       </c>
-      <c r="AV21" t="s">
+      <c r="AN24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO24">
+        <v>0</v>
+      </c>
+      <c r="AP24">
+        <v>13</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR24" t="s">
+        <v>246</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>389</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>390</v>
+      </c>
+      <c r="AV24" t="s">
         <v>107</v>
       </c>
-      <c r="AW21" t="s">
+      <c r="AW24" t="s">
         <v>165</v>
       </c>
-      <c r="AY21" t="s">
-        <v>389</v>
-      </c>
-      <c r="BA21" t="s">
+      <c r="AY24" t="s">
+        <v>391</v>
+      </c>
+      <c r="BA24" t="s">
         <v>167</v>
       </c>
-      <c r="BC21" t="s">
+      <c r="BC24" t="s">
         <v>72</v>
       </c>
-      <c r="BD21">
+      <c r="BD24">
         <v>239</v>
       </c>
-      <c r="BE21">
+      <c r="BE24">
         <v>20</v>
       </c>
-      <c r="BF21">
+      <c r="BF24">
         <v>45</v>
       </c>
-      <c r="BI21" t="s">
+      <c r="BI24" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4343,87 +4367,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="AM1:BJ1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="39:62">
-      <c r="AM1" t="s">
-        <v>390</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>391</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>392</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>393</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>394</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>395</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>396</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>397</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>398</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>399</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>400</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>401</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>402</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>403</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>404</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>405</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>406</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>407</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>408</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>409</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>410</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>411</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>412</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>